<commit_message>
implementing data driver for API tests
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/TestData.xlsx
+++ b/src/test/resources/Data/TestData.xlsx
@@ -3,32 +3,24 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F502F0-1DFC-42B3-BC33-0E09E302697E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E3C37C8-1BE6-4BE3-85F0-E901CDA67D22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="GoogleTest" sheetId="1" r:id="rId1"/>
+    <sheet name="UiTestData" sheetId="1" r:id="rId1"/>
+    <sheet name="ApiTestData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>TestName</t>
   </si>
   <si>
-    <t>SearchKey</t>
-  </si>
-  <si>
-    <t>TC001</t>
-  </si>
-  <si>
-    <t>TC002</t>
-  </si>
-  <si>
     <t>test</t>
   </si>
   <si>
@@ -39,13 +31,60 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>UITC-001</t>
+  </si>
+  <si>
+    <t>UITC-002</t>
+  </si>
+  <si>
+    <t>APITC-001</t>
+  </si>
+  <si>
+    <t>APITC-002</t>
+  </si>
+  <si>
+    <t>EndPoint</t>
+  </si>
+  <si>
+    <t>StatusCode</t>
+  </si>
+  <si>
+    <r>
+      <t>/us</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006400"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>90210</t>
+    </r>
+  </si>
+  <si>
+    <t>400</t>
+  </si>
+  <si>
+    <t>200</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -53,13 +92,45 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF8B0000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006400"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -74,8 +145,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -425,42 +511,111 @@
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC22D428-483B-4047-B6E1-9C9F7C1A7C42}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="4" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>